<commit_message>
feat: Complete sample data verification with interactive step-by-step process
- Reorganized sample_data to flat structure matching production
- Added comprehensive verification scripts (verify_interactive.py, run_step.py)
- Created sample_data_run_verification.md documentation
- Updated CLAUDE.md with mandatory file naming conventions
- Enhanced data validation with reference metadata tables
- All 6 verification steps completed successfully
</commit_message>
<xml_diff>
--- a/specs/modules/fatigue-analysis/reference-seastate-scaling-fatigue/input/reference_seastates.xlsx
+++ b/specs/modules/fatigue-analysis/reference-seastate-scaling-fatigue/input/reference_seastates.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\Acma-ansys05\D\github\digitalmodel\specs\modules\fatigue-analysis\strut-foundation-rainflow\input\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\Acma-ansys05\D\github\digitalmodel\specs\modules\fatigue-analysis\reference-seastate-scaling-fatigue\input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2788402E-E7FD-4E03-8B86-BDAE3A8CA8D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72D2634B-8793-48B4-9CE9-83465AFFF571}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="15000" activeTab="3" xr2:uid="{213788C7-1522-40E6-BF85-9ADB5F321826}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="15000" activeTab="2" xr2:uid="{213788C7-1522-40E6-BF85-9ADB5F321826}"/>
   </bookViews>
   <sheets>
     <sheet name="reference" sheetId="1" r:id="rId1"/>
@@ -14365,8 +14365,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{07F2B15F-1B76-435F-9F2E-D653FC573605}">
   <dimension ref="A1:B502"/>
   <sheetViews>
-    <sheetView topLeftCell="A470" workbookViewId="0">
-      <selection sqref="A1:B502"/>
+    <sheetView tabSelected="1" topLeftCell="A137" workbookViewId="0">
+      <selection activeCell="B151" sqref="B151"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -18890,7 +18890,7 @@
     </row>
     <row r="453" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A453">
-        <f t="shared" ref="A453:A516" si="14">A452+4</f>
+        <f t="shared" ref="A453:A502" si="14">A452+4</f>
         <v>1804</v>
       </c>
       <c r="B453">
@@ -19397,8 +19397,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9958FC15-73ED-40D0-8DFE-AB10240E50C2}">
   <dimension ref="A1:C9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:B9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>